<commit_message>
Updated printing behavior and button cost estimate
</commit_message>
<xml_diff>
--- a/Generate Cost Function.xlsx
+++ b/Generate Cost Function.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtsou\Projects\twiddler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C7D2B6-3A8E-4A18-B5B4-DEA4D7508CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DA638D-AC02-4160-8973-E712161DB8BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA8A9BB7-B18C-4F11-9B65-65D3E17F7E9C}"/>
   </bookViews>
@@ -33,8 +33,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={3B7CF826-4BCE-4B7E-A9FF-FA9F725A8D2D}</author>
+  </authors>
+  <commentList>
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{3B7CF826-4BCE-4B7E-A9FF-FA9F725A8D2D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Muliple buttons per row increased to match pinky (MR), because that was the only trained multiple buttons per row.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Left</t>
   </si>
@@ -100,6 +118,9 @@
 Count the total, mispresses have a penalty of -1.
 Home row keys have there count halfed since the finger doesn't need to return to home between presses.</t>
   </si>
+  <si>
+    <t>10/24/2020 - Adjusted</t>
+  </si>
 </sst>
 </file>
 
@@ -108,7 +129,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +144,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -183,11 +210,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -219,6 +287,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jared Soundy" id="{67EB4A80-5E01-4F50-82D4-EF8E3CA40201}" userId="8612722642432b0e" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -516,12 +590,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="R2" dT="2020-10-24T15:39:03.50" personId="{67EB4A80-5E01-4F50-82D4-EF8E3CA40201}" id="{3B7CF826-4BCE-4B7E-A9FF-FA9F725A8D2D}">
+    <text>Muliple buttons per row increased to match pinky (MR), because that was the only trained multiple buttons per row.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842575C2-51D4-422F-A3B2-83CACC094C40}">
   <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E5" sqref="E5:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,9 +613,12 @@
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.140625" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="18" width="18" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="10" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1"/>
+    <col min="7" max="15" width="18" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="29.42578125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="23.140625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="23.85546875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -719,11 +804,11 @@
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>"If(G[i] &amp; P[" &amp; C5 &amp; "] == P[" &amp; C5 &amp; "], " &amp; AF5 &amp; " / len(n_gram[i]), " &amp; S5</f>
-        <v>If(G[i] &amp; P[0] == P[0], 1.875 / len(n_gram[i]), #  000 000 000 110</v>
+        <v>If(G[i] &amp; P[0] == P[0], 1.53846153846154 / len(n_gram[i]), #  000 000 011 000</v>
       </c>
       <c r="B5" t="str">
         <f>"s.add(P[" &amp; C5 &amp; "] == " &amp; D5 &amp; ") " &amp; S5</f>
-        <v>s.add(P[0] == 6) #  000 000 000 110</v>
+        <v>s.add(P[0] == 24) #  000 000 011 000</v>
       </c>
       <c r="C5">
         <f>C4+1</f>
@@ -731,15 +816,15 @@
       </c>
       <c r="D5" s="3">
         <f>T5*$T$1+U5*$U$1+V5*$V$1+W5*$W$1+X5*$X$1+Y5*$Y$1+Z5*$Z$1+AA5*$AA$1+AB5*$AB$1+AC5*$AC$1+AD5*$AD$1+AE5</f>
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E5" t="str">
         <f>"If(" &amp; IF(SUM(T5:AE5) &gt; 1, "And(" &amp; F5 &amp; ")", F5) &amp; ",  " &amp; AF5 &amp; " / len(n.grams[i]), " &amp; S5</f>
-        <v>If(And(Extract(2, 2, b.G[i]) == 1, Extract(1, 1, b.G[i]) == 1),  1.875 / len(n.grams[i]), #  000 000 000 110</v>
+        <v>If(And(Extract(4, 4, b.G[i]) == 1, Extract(3, 3, b.G[i]) == 1),  1.53846153846154 / len(n.grams[i]), #  000 000 011 000</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F24" si="1">G5 &amp; H5 &amp; I5 &amp; J5 &amp; K5 &amp; L5 &amp; M5 &amp; N5 &amp; O5 &amp; P5 &amp; Q5 &amp; R5</f>
-        <v>Extract(2, 2, b.G[i]) == 1, Extract(1, 1, b.G[i]) == 1</v>
+        <f>G5 &amp; H5 &amp; I5 &amp; J5 &amp; K5 &amp; L5 &amp; M5 &amp; N5 &amp; O5 &amp; P5 &amp; Q5 &amp; R5</f>
+        <v>Extract(4, 4, b.G[i]) == 1, Extract(3, 3, b.G[i]) == 1</v>
       </c>
       <c r="G5" t="str">
         <f>IF(T5&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U5:$AE5) &gt; 0,", ",""), "")</f>
@@ -771,27 +856,27 @@
       </c>
       <c r="N5" t="str">
         <f>IF(AA5&gt;0,"Extract(" &amp; AA$2 &amp; ", " &amp; AA$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AB5:$AE5) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v xml:space="preserve">Extract(4, 4, b.G[i]) == 1, </v>
       </c>
       <c r="O5" t="str">
         <f>IF(AB5&gt;0,"Extract(" &amp; AB$2 &amp; ", " &amp; AB$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AC5:$AE5) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(3, 3, b.G[i]) == 1</v>
       </c>
       <c r="P5" t="str">
         <f>IF(AC5&gt;0,"Extract(" &amp; AC$2 &amp; ", " &amp; AC$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AD5:$AE5) &gt; 0,", ",""), "")</f>
-        <v xml:space="preserve">Extract(2, 2, b.G[i]) == 1, </v>
+        <v/>
       </c>
       <c r="Q5" t="str">
         <f>IF(AD5&gt;0,"Extract(" &amp; AD$2 &amp; ", " &amp; AD$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AE5:$AE5) &gt; 0,", ",""), "")</f>
-        <v>Extract(1, 1, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="R5" t="str">
-        <f>IF(AE5&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE5:AF5) &gt; 0,", ",""), "")</f>
+        <f>IF(AE5&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1", "")</f>
         <v/>
       </c>
       <c r="S5" t="str">
-        <f t="shared" ref="S5:S24" si="2">"#  " &amp; T5 &amp; U5 &amp; V5 &amp; " " &amp; W5 &amp; X5 &amp; Y5 &amp; " " &amp; Z5 &amp; AA5 &amp; AB5 &amp; " " &amp; AC5 &amp; AD5 &amp; AE5</f>
-        <v>#  000 000 000 110</v>
+        <f>"#  " &amp; T5 &amp; U5 &amp; V5 &amp; " " &amp; W5 &amp; X5 &amp; Y5 &amp; " " &amp; Z5 &amp; AA5 &amp; AB5 &amp; " " &amp; AC5 &amp; AD5 &amp; AE5</f>
+        <v>#  000 000 011 000</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -815,52 +900,52 @@
         <v>0</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5">
         <v>0</v>
       </c>
       <c r="AF5" s="2">
-        <v>1.875</v>
+        <v>1.5384615384615385</v>
       </c>
       <c r="AG5">
-        <f t="shared" ref="AG5:AG24" si="3">COUNTIF(T5:AE5,"&gt;0")</f>
+        <f>COUNTIF(T5:AE5,"&gt;0")</f>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f t="shared" ref="A6:A24" si="4">"If(G[i] &amp; P[" &amp; C6 &amp; "] == P[" &amp; C6 &amp; "], " &amp; AF6 &amp; " / len(n_gram[i]), " &amp; S6</f>
-        <v>If(G[i] &amp; P[1] == P[1], 1.66666666666667 / len(n_gram[i]), #  000 000 011 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C6 &amp; "] == P[" &amp; C6 &amp; "], " &amp; AF6 &amp; " / len(n_gram[i]), " &amp; S6</f>
+        <v>If(G[i] &amp; P[1] == P[1], 1.53846153846154 / len(n_gram[i]), #  000 000 110 000</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" ref="B6:B24" si="5">"s.add(P[" &amp; C6 &amp; "] == " &amp; D6 &amp; ") " &amp; S6</f>
-        <v>s.add(P[1] == 24) #  000 000 011 000</v>
+        <f>"s.add(P[" &amp; C6 &amp; "] == " &amp; D6 &amp; ") " &amp; S6</f>
+        <v>s.add(P[1] == 48) #  000 000 110 000</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:C24" si="6">C5+1</f>
+        <f>C5+1</f>
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" ref="D6:D24" si="7">T6*$T$1+U6*$U$1+V6*$V$1+W6*$W$1+X6*$X$1+Y6*$Y$1+Z6*$Z$1+AA6*$AA$1+AB6*$AB$1+AC6*$AC$1+AD6*$AD$1+AE6</f>
-        <v>24</v>
+        <f>T6*$T$1+U6*$U$1+V6*$V$1+W6*$W$1+X6*$X$1+Y6*$Y$1+Z6*$Z$1+AA6*$AA$1+AB6*$AB$1+AC6*$AC$1+AD6*$AD$1+AE6</f>
+        <v>48</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" ref="E6:E24" si="8">"If(" &amp; IF(SUM(T6:AE6) &gt; 1, "And(" &amp; F6 &amp; ")", F6) &amp; ",  " &amp; AF6 &amp; " / len(n.grams[i]), " &amp; S6</f>
-        <v>If(And(Extract(4, 4, b.G[i]) == 1, Extract(3, 3, b.G[i]) == 1),  1.66666666666667 / len(n.grams[i]), #  000 000 011 000</v>
+        <f t="shared" ref="E6:E24" si="1">"If(" &amp; IF(SUM(T6:AE6) &gt; 1, "And(" &amp; F6 &amp; ")", F6) &amp; ",  " &amp; AF6 &amp; " / len(n.grams[i]), " &amp; S6</f>
+        <v>If(And(Extract(5, 5, b.G[i]) == 1, Extract(4, 4, b.G[i]) == 1),  1.53846153846154 / len(n.grams[i]), #  000 000 110 000</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(4, 4, b.G[i]) == 1, Extract(3, 3, b.G[i]) == 1</v>
+        <f>G6 &amp; H6 &amp; I6 &amp; J6 &amp; K6 &amp; L6 &amp; M6 &amp; N6 &amp; O6 &amp; P6 &amp; Q6 &amp; R6</f>
+        <v>Extract(5, 5, b.G[i]) == 1, Extract(4, 4, b.G[i]) == 1</v>
       </c>
       <c r="G6" t="str">
         <f>IF(T6&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U6:$AE6) &gt; 0,", ",""), "")</f>
@@ -888,15 +973,15 @@
       </c>
       <c r="M6" t="str">
         <f>IF(Z6&gt;0,"Extract(" &amp; Z$2 &amp; ", " &amp; Z$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AA6:$AE6) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v xml:space="preserve">Extract(5, 5, b.G[i]) == 1, </v>
       </c>
       <c r="N6" t="str">
         <f>IF(AA6&gt;0,"Extract(" &amp; AA$2 &amp; ", " &amp; AA$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AB6:$AE6) &gt; 0,", ",""), "")</f>
-        <v xml:space="preserve">Extract(4, 4, b.G[i]) == 1, </v>
+        <v>Extract(4, 4, b.G[i]) == 1</v>
       </c>
       <c r="O6" t="str">
         <f>IF(AB6&gt;0,"Extract(" &amp; AB$2 &amp; ", " &amp; AB$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AC6:$AE6) &gt; 0,", ",""), "")</f>
-        <v>Extract(3, 3, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="P6" t="str">
         <f>IF(AC6&gt;0,"Extract(" &amp; AC$2 &amp; ", " &amp; AC$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AD6:$AE6) &gt; 0,", ",""), "")</f>
@@ -907,12 +992,12 @@
         <v/>
       </c>
       <c r="R6" t="str">
-        <f>IF(AE6&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE6:AF6) &gt; 0,", ",""), "")</f>
+        <f t="shared" ref="R6:R24" si="2">IF(AE6&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1", "")</f>
         <v/>
       </c>
       <c r="S6" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 000 011 000</v>
+        <f>"#  " &amp; T6 &amp; U6 &amp; V6 &amp; " " &amp; W6 &amp; X6 &amp; Y6 &amp; " " &amp; Z6 &amp; AA6 &amp; AB6 &amp; " " &amp; AC6 &amp; AD6 &amp; AE6</f>
+        <v>#  000 000 110 000</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -933,13 +1018,13 @@
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6">
         <v>1</v>
       </c>
       <c r="AB6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -951,37 +1036,37 @@
         <v>0</v>
       </c>
       <c r="AF6" s="2">
-        <v>1.6666666666666667</v>
+        <v>1.5384615384615385</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T6:AE6,"&gt;0")</f>
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[2] == P[2], 1.62162162162162 / len(n_gram[i]), #  000 011 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C7 &amp; "] == P[" &amp; C7 &amp; "], " &amp; AF7 &amp; " / len(n_gram[i]), " &amp; S7</f>
+        <v>If(G[i] &amp; P[2] == P[2], 1.53846153846154 / len(n_gram[i]), #  000 000 000 011</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[2] == 192) #  000 011 000 000</v>
+        <f>"s.add(P[" &amp; C7 &amp; "] == " &amp; D7 &amp; ") " &amp; S7</f>
+        <v>s.add(P[2] == 3) #  000 000 000 011</v>
       </c>
       <c r="C7">
-        <f t="shared" si="6"/>
+        <f>C6+1</f>
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="7"/>
-        <v>192</v>
+        <f>T7*$T$1+U7*$U$1+V7*$V$1+W7*$W$1+X7*$X$1+Y7*$Y$1+Z7*$Z$1+AA7*$AA$1+AB7*$AB$1+AC7*$AC$1+AD7*$AD$1+AE7</f>
+        <v>3</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="8"/>
-        <v>If(And(Extract(7, 7, b.G[i]) == 1, Extract(6, 6, b.G[i]) == 1),  1.62162162162162 / len(n.grams[i]), #  000 011 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(And(Extract(1, 1, b.G[i]) == 1, Extract(0, 0, b.G[i]) == 1),  1.53846153846154 / len(n.grams[i]), #  000 000 000 011</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(7, 7, b.G[i]) == 1, Extract(6, 6, b.G[i]) == 1</v>
+        <f>G7 &amp; H7 &amp; I7 &amp; J7 &amp; K7 &amp; L7 &amp; M7 &amp; N7 &amp; O7 &amp; P7 &amp; Q7 &amp; R7</f>
+        <v>Extract(1, 1, b.G[i]) == 1, Extract(0, 0, b.G[i]) == 1</v>
       </c>
       <c r="G7" t="str">
         <f>IF(T7&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U7:$AE7) &gt; 0,", ",""), "")</f>
@@ -1001,11 +1086,11 @@
       </c>
       <c r="K7" t="str">
         <f>IF(X7&gt;0,"Extract(" &amp; X$2 &amp; ", " &amp; X$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Y7:$AE7) &gt; 0,", ",""), "")</f>
-        <v xml:space="preserve">Extract(7, 7, b.G[i]) == 1, </v>
+        <v/>
       </c>
       <c r="L7" t="str">
         <f>IF(Y7&gt;0,"Extract(" &amp; Y$2 &amp; ", " &amp; Y$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Z7:$AE7) &gt; 0,", ",""), "")</f>
-        <v>Extract(6, 6, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="M7" t="str">
         <f>IF(Z7&gt;0,"Extract(" &amp; Z$2 &amp; ", " &amp; Z$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AA7:$AE7) &gt; 0,", ",""), "")</f>
@@ -1025,15 +1110,15 @@
       </c>
       <c r="Q7" t="str">
         <f>IF(AD7&gt;0,"Extract(" &amp; AD$2 &amp; ", " &amp; AD$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AE7:$AE7) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v xml:space="preserve">Extract(1, 1, b.G[i]) == 1, </v>
       </c>
       <c r="R7" t="str">
-        <f>IF(AE7&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE7:AF7) &gt; 0,", ",""), "")</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>Extract(0, 0, b.G[i]) == 1</v>
       </c>
       <c r="S7" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 011 000 000</v>
+        <f>"#  " &amp; T7 &amp; U7 &amp; V7 &amp; " " &amp; W7 &amp; X7 &amp; Y7 &amp; " " &amp; Z7 &amp; AA7 &amp; AB7 &amp; " " &amp; AC7 &amp; AD7 &amp; AE7</f>
+        <v>#  000 000 000 011</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -1048,10 +1133,10 @@
         <v>0</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z7">
         <v>0</v>
@@ -1066,43 +1151,43 @@
         <v>0</v>
       </c>
       <c r="AD7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7" s="2">
-        <v>1.6216216216216217</v>
+        <v>1.5384615384615385</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T7:AE7,"&gt;0")</f>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[3] == P[3], 1.46341463414634 / len(n_gram[i]), #  000 000 110 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C8 &amp; "] == P[" &amp; C8 &amp; "], " &amp; AF8 &amp; " / len(n_gram[i]), " &amp; S8</f>
+        <v>If(G[i] &amp; P[3] == P[3], 1.53846153846154 / len(n_gram[i]), #  000 000 000 110</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[3] == 48) #  000 000 110 000</v>
+        <f>"s.add(P[" &amp; C8 &amp; "] == " &amp; D8 &amp; ") " &amp; S8</f>
+        <v>s.add(P[3] == 6) #  000 000 000 110</v>
       </c>
       <c r="C8">
-        <f t="shared" si="6"/>
+        <f>C7+1</f>
         <v>3</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="7"/>
-        <v>48</v>
+        <f>T8*$T$1+U8*$U$1+V8*$V$1+W8*$W$1+X8*$X$1+Y8*$Y$1+Z8*$Z$1+AA8*$AA$1+AB8*$AB$1+AC8*$AC$1+AD8*$AD$1+AE8</f>
+        <v>6</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="8"/>
-        <v>If(And(Extract(5, 5, b.G[i]) == 1, Extract(4, 4, b.G[i]) == 1),  1.46341463414634 / len(n.grams[i]), #  000 000 110 000</v>
+        <f t="shared" si="1"/>
+        <v>If(And(Extract(2, 2, b.G[i]) == 1, Extract(1, 1, b.G[i]) == 1),  1.53846153846154 / len(n.grams[i]), #  000 000 000 110</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(5, 5, b.G[i]) == 1, Extract(4, 4, b.G[i]) == 1</v>
+        <f>G8 &amp; H8 &amp; I8 &amp; J8 &amp; K8 &amp; L8 &amp; M8 &amp; N8 &amp; O8 &amp; P8 &amp; Q8 &amp; R8</f>
+        <v>Extract(2, 2, b.G[i]) == 1, Extract(1, 1, b.G[i]) == 1</v>
       </c>
       <c r="G8" t="str">
         <f>IF(T8&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U8:$AE8) &gt; 0,", ",""), "")</f>
@@ -1130,11 +1215,11 @@
       </c>
       <c r="M8" t="str">
         <f>IF(Z8&gt;0,"Extract(" &amp; Z$2 &amp; ", " &amp; Z$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AA8:$AE8) &gt; 0,", ",""), "")</f>
-        <v xml:space="preserve">Extract(5, 5, b.G[i]) == 1, </v>
+        <v/>
       </c>
       <c r="N8" t="str">
         <f>IF(AA8&gt;0,"Extract(" &amp; AA$2 &amp; ", " &amp; AA$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AB8:$AE8) &gt; 0,", ",""), "")</f>
-        <v>Extract(4, 4, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="O8" t="str">
         <f>IF(AB8&gt;0,"Extract(" &amp; AB$2 &amp; ", " &amp; AB$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AC8:$AE8) &gt; 0,", ",""), "")</f>
@@ -1142,19 +1227,19 @@
       </c>
       <c r="P8" t="str">
         <f>IF(AC8&gt;0,"Extract(" &amp; AC$2 &amp; ", " &amp; AC$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AD8:$AE8) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v xml:space="preserve">Extract(2, 2, b.G[i]) == 1, </v>
       </c>
       <c r="Q8" t="str">
         <f>IF(AD8&gt;0,"Extract(" &amp; AD$2 &amp; ", " &amp; AD$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AE8:$AE8) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(1, 1, b.G[i]) == 1</v>
       </c>
       <c r="R8" t="str">
-        <f>IF(AE8&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE8:AF8) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S8" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 000 110 000</v>
+        <f>"#  " &amp; T8 &amp; U8 &amp; V8 &amp; " " &amp; W8 &amp; X8 &amp; Y8 &amp; " " &amp; Z8 &amp; AA8 &amp; AB8 &amp; " " &amp; AC8 &amp; AD8 &amp; AE8</f>
+        <v>#  000 000 000 110</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -1175,63 +1260,63 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB8">
         <v>0</v>
       </c>
       <c r="AC8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE8">
         <v>0</v>
       </c>
       <c r="AF8" s="2">
-        <v>1.4634146341463414</v>
+        <v>1.5384615384615385</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T8:AE8,"&gt;0")</f>
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[4] == P[4], 1.42857142857143 / len(n_gram[i]), #  000 110 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C9 &amp; "] == P[" &amp; C9 &amp; "], " &amp; AF9 &amp; " / len(n_gram[i]), " &amp; S9</f>
+        <v>If(G[i] &amp; P[4] == P[4], 1.27659574468085 / len(n_gram[i]), #  110 000 000 000</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[4] == 384) #  000 110 000 000</v>
+        <f>"s.add(P[" &amp; C9 &amp; "] == " &amp; D9 &amp; ") " &amp; S9</f>
+        <v>s.add(P[4] == 3072) #  110 000 000 000</v>
       </c>
       <c r="C9">
-        <f t="shared" si="6"/>
+        <f>C8+1</f>
         <v>4</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="7"/>
-        <v>384</v>
+        <f>T9*$T$1+U9*$U$1+V9*$V$1+W9*$W$1+X9*$X$1+Y9*$Y$1+Z9*$Z$1+AA9*$AA$1+AB9*$AB$1+AC9*$AC$1+AD9*$AD$1+AE9</f>
+        <v>3072</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="8"/>
-        <v>If(And(Extract(8, 8, b.G[i]) == 1, Extract(7, 7, b.G[i]) == 1),  1.42857142857143 / len(n.grams[i]), #  000 110 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(And(Extract(11, 11, b.G[i]) == 1, Extract(10, 10, b.G[i]) == 1),  1.27659574468085 / len(n.grams[i]), #  110 000 000 000</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(8, 8, b.G[i]) == 1, Extract(7, 7, b.G[i]) == 1</v>
+        <f>G9 &amp; H9 &amp; I9 &amp; J9 &amp; K9 &amp; L9 &amp; M9 &amp; N9 &amp; O9 &amp; P9 &amp; Q9 &amp; R9</f>
+        <v>Extract(11, 11, b.G[i]) == 1, Extract(10, 10, b.G[i]) == 1</v>
       </c>
       <c r="G9" t="str">
         <f>IF(T9&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U9:$AE9) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v xml:space="preserve">Extract(11, 11, b.G[i]) == 1, </v>
       </c>
       <c r="H9" t="str">
         <f>IF(U9&gt;0,"Extract(" &amp; U$2 &amp; ", " &amp; U$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(V9:$AE9) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(10, 10, b.G[i]) == 1</v>
       </c>
       <c r="I9" t="str">
         <f>IF(V9&gt;0,"Extract(" &amp; V$2 &amp; ", " &amp; V$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(W9:$AE9) &gt; 0,", ",""), "")</f>
@@ -1239,11 +1324,11 @@
       </c>
       <c r="J9" t="str">
         <f>IF(W9&gt;0,"Extract(" &amp; W$2 &amp; ", " &amp; W$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(X9:$AE9) &gt; 0,", ",""), "")</f>
-        <v xml:space="preserve">Extract(8, 8, b.G[i]) == 1, </v>
+        <v/>
       </c>
       <c r="K9" t="str">
         <f>IF(X9&gt;0,"Extract(" &amp; X$2 &amp; ", " &amp; X$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Y9:$AE9) &gt; 0,", ",""), "")</f>
-        <v>Extract(7, 7, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="L9" t="str">
         <f>IF(Y9&gt;0,"Extract(" &amp; Y$2 &amp; ", " &amp; Y$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Z9:$AE9) &gt; 0,", ",""), "")</f>
@@ -1270,27 +1355,27 @@
         <v/>
       </c>
       <c r="R9" t="str">
-        <f>IF(AE9&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE9:AF9) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S9" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 110 000 000</v>
+        <f>"#  " &amp; T9 &amp; U9 &amp; V9 &amp; " " &amp; W9 &amp; X9 &amp; Y9 &amp; " " &amp; Z9 &amp; AA9 &amp; AB9 &amp; " " &amp; AC9 &amp; AD9 &amp; AE9</f>
+        <v>#  110 000 000 000</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <v>0</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -1314,37 +1399,37 @@
         <v>0</v>
       </c>
       <c r="AF9" s="2">
-        <v>1.4285714285714286</v>
+        <v>1.2765957446808511</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T9:AE9,"&gt;0")</f>
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[5] == P[5], 1.36363636363636 / len(n_gram[i]), #  000 000 000 011</v>
+        <f>"If(G[i] &amp; P[" &amp; C10 &amp; "] == P[" &amp; C10 &amp; "], " &amp; AF10 &amp; " / len(n_gram[i]), " &amp; S10</f>
+        <v>If(G[i] &amp; P[5] == P[5], 1.2 / len(n_gram[i]), #  000 110 000 000</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[5] == 3) #  000 000 000 011</v>
+        <f>"s.add(P[" &amp; C10 &amp; "] == " &amp; D10 &amp; ") " &amp; S10</f>
+        <v>s.add(P[5] == 384) #  000 110 000 000</v>
       </c>
       <c r="C10">
-        <f t="shared" si="6"/>
+        <f>C9+1</f>
         <v>5</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="7"/>
-        <v>3</v>
+        <f>T10*$T$1+U10*$U$1+V10*$V$1+W10*$W$1+X10*$X$1+Y10*$Y$1+Z10*$Z$1+AA10*$AA$1+AB10*$AB$1+AC10*$AC$1+AD10*$AD$1+AE10</f>
+        <v>384</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="8"/>
-        <v>If(And(Extract(1, 1, b.G[i]) == 1, Extract(0, 0, b.G[i]) == 1, ),  1.36363636363636 / len(n.grams[i]), #  000 000 000 011</v>
+        <f t="shared" si="1"/>
+        <v>If(And(Extract(8, 8, b.G[i]) == 1, Extract(7, 7, b.G[i]) == 1),  1.2 / len(n.grams[i]), #  000 110 000 000</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">Extract(1, 1, b.G[i]) == 1, Extract(0, 0, b.G[i]) == 1, </v>
+        <f>G10 &amp; H10 &amp; I10 &amp; J10 &amp; K10 &amp; L10 &amp; M10 &amp; N10 &amp; O10 &amp; P10 &amp; Q10 &amp; R10</f>
+        <v>Extract(8, 8, b.G[i]) == 1, Extract(7, 7, b.G[i]) == 1</v>
       </c>
       <c r="G10" t="str">
         <f>IF(T10&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U10:$AE10) &gt; 0,", ",""), "")</f>
@@ -1360,11 +1445,11 @@
       </c>
       <c r="J10" t="str">
         <f>IF(W10&gt;0,"Extract(" &amp; W$2 &amp; ", " &amp; W$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(X10:$AE10) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v xml:space="preserve">Extract(8, 8, b.G[i]) == 1, </v>
       </c>
       <c r="K10" t="str">
         <f>IF(X10&gt;0,"Extract(" &amp; X$2 &amp; ", " &amp; X$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Y10:$AE10) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(7, 7, b.G[i]) == 1</v>
       </c>
       <c r="L10" t="str">
         <f>IF(Y10&gt;0,"Extract(" &amp; Y$2 &amp; ", " &amp; Y$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Z10:$AE10) &gt; 0,", ",""), "")</f>
@@ -1388,15 +1473,15 @@
       </c>
       <c r="Q10" t="str">
         <f>IF(AD10&gt;0,"Extract(" &amp; AD$2 &amp; ", " &amp; AD$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AE10:$AE10) &gt; 0,", ",""), "")</f>
-        <v xml:space="preserve">Extract(1, 1, b.G[i]) == 1, </v>
+        <v/>
       </c>
       <c r="R10" t="str">
-        <f>IF(AE10&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE10:AF10) &gt; 0,", ",""), "")</f>
-        <v xml:space="preserve">Extract(0, 0, b.G[i]) == 1, </v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="S10" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 000 000 011</v>
+        <f>"#  " &amp; T10 &amp; U10 &amp; V10 &amp; " " &amp; W10 &amp; X10 &amp; Y10 &amp; " " &amp; Z10 &amp; AA10 &amp; AB10 &amp; " " &amp; AC10 &amp; AD10 &amp; AE10</f>
+        <v>#  000 110 000 000</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -1408,10 +1493,10 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -1429,51 +1514,51 @@
         <v>0</v>
       </c>
       <c r="AD10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF10" s="2">
-        <v>1.3636363636363635</v>
+        <v>1.2</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T10:AE10,"&gt;0")</f>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[6] == P[6], 1.27659574468085 / len(n_gram[i]), #  110 000 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C11 &amp; "] == P[" &amp; C11 &amp; "], " &amp; AF11 &amp; " / len(n_gram[i]), " &amp; S11</f>
+        <v>If(G[i] &amp; P[6] == P[6], 1.11111111111111 / len(n_gram[i]), #  000 011 000 000</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[6] == 3072) #  110 000 000 000</v>
+        <f>"s.add(P[" &amp; C11 &amp; "] == " &amp; D11 &amp; ") " &amp; S11</f>
+        <v>s.add(P[6] == 192) #  000 011 000 000</v>
       </c>
       <c r="C11">
-        <f t="shared" si="6"/>
+        <f>C10+1</f>
         <v>6</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="7"/>
-        <v>3072</v>
+        <f>T11*$T$1+U11*$U$1+V11*$V$1+W11*$W$1+X11*$X$1+Y11*$Y$1+Z11*$Z$1+AA11*$AA$1+AB11*$AB$1+AC11*$AC$1+AD11*$AD$1+AE11</f>
+        <v>192</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="8"/>
-        <v>If(And(Extract(11, 11, b.G[i]) == 1, Extract(10, 10, b.G[i]) == 1),  1.27659574468085 / len(n.grams[i]), #  110 000 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(And(Extract(7, 7, b.G[i]) == 1, Extract(6, 6, b.G[i]) == 1),  1.11111111111111 / len(n.grams[i]), #  000 011 000 000</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(11, 11, b.G[i]) == 1, Extract(10, 10, b.G[i]) == 1</v>
+        <f>G11 &amp; H11 &amp; I11 &amp; J11 &amp; K11 &amp; L11 &amp; M11 &amp; N11 &amp; O11 &amp; P11 &amp; Q11 &amp; R11</f>
+        <v>Extract(7, 7, b.G[i]) == 1, Extract(6, 6, b.G[i]) == 1</v>
       </c>
       <c r="G11" t="str">
         <f>IF(T11&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U11:$AE11) &gt; 0,", ",""), "")</f>
-        <v xml:space="preserve">Extract(11, 11, b.G[i]) == 1, </v>
+        <v/>
       </c>
       <c r="H11" t="str">
         <f>IF(U11&gt;0,"Extract(" &amp; U$2 &amp; ", " &amp; U$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(V11:$AE11) &gt; 0,", ",""), "")</f>
-        <v>Extract(10, 10, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="I11" t="str">
         <f>IF(V11&gt;0,"Extract(" &amp; V$2 &amp; ", " &amp; V$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(W11:$AE11) &gt; 0,", ",""), "")</f>
@@ -1485,11 +1570,11 @@
       </c>
       <c r="K11" t="str">
         <f>IF(X11&gt;0,"Extract(" &amp; X$2 &amp; ", " &amp; X$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Y11:$AE11) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v xml:space="preserve">Extract(7, 7, b.G[i]) == 1, </v>
       </c>
       <c r="L11" t="str">
         <f>IF(Y11&gt;0,"Extract(" &amp; Y$2 &amp; ", " &amp; Y$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Z11:$AE11) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(6, 6, b.G[i]) == 1</v>
       </c>
       <c r="M11" t="str">
         <f>IF(Z11&gt;0,"Extract(" &amp; Z$2 &amp; ", " &amp; Z$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AA11:$AE11) &gt; 0,", ",""), "")</f>
@@ -1512,18 +1597,18 @@
         <v/>
       </c>
       <c r="R11" t="str">
-        <f>IF(AE11&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE11:AF11) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S11" t="str">
-        <f t="shared" si="2"/>
-        <v>#  110 000 000 000</v>
+        <f>"#  " &amp; T11 &amp; U11 &amp; V11 &amp; " " &amp; W11 &amp; X11 &amp; Y11 &amp; " " &amp; Z11 &amp; AA11 &amp; AB11 &amp; " " &amp; AC11 &amp; AD11 &amp; AE11</f>
+        <v>#  000 011 000 000</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -1532,10 +1617,10 @@
         <v>0</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11">
         <v>0</v>
@@ -1556,36 +1641,36 @@
         <v>0</v>
       </c>
       <c r="AF11" s="2">
-        <v>1.2765957446808511</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T11:AE11,"&gt;0")</f>
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[7] == P[7], 1.15384615384615 / len(n_gram[i]), #  011 000 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C12 &amp; "] == P[" &amp; C12 &amp; "], " &amp; AF12 &amp; " / len(n_gram[i]), " &amp; S12</f>
+        <v>If(G[i] &amp; P[7] == P[7], 1.09090909090909 / len(n_gram[i]), #  011 000 000 000</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="5"/>
+        <f>"s.add(P[" &amp; C12 &amp; "] == " &amp; D12 &amp; ") " &amp; S12</f>
         <v>s.add(P[7] == 1536) #  011 000 000 000</v>
       </c>
       <c r="C12">
-        <f t="shared" si="6"/>
+        <f>C11+1</f>
         <v>7</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="7"/>
+        <f>T12*$T$1+U12*$U$1+V12*$V$1+W12*$W$1+X12*$X$1+Y12*$Y$1+Z12*$Z$1+AA12*$AA$1+AB12*$AB$1+AC12*$AC$1+AD12*$AD$1+AE12</f>
         <v>1536</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="8"/>
-        <v>If(And(Extract(10, 10, b.G[i]) == 1, Extract(9, 9, b.G[i]) == 1),  1.15384615384615 / len(n.grams[i]), #  011 000 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(And(Extract(10, 10, b.G[i]) == 1, Extract(9, 9, b.G[i]) == 1),  1.09090909090909 / len(n.grams[i]), #  011 000 000 000</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="1"/>
+        <f>G12 &amp; H12 &amp; I12 &amp; J12 &amp; K12 &amp; L12 &amp; M12 &amp; N12 &amp; O12 &amp; P12 &amp; Q12 &amp; R12</f>
         <v>Extract(10, 10, b.G[i]) == 1, Extract(9, 9, b.G[i]) == 1</v>
       </c>
       <c r="G12" t="str">
@@ -1633,11 +1718,11 @@
         <v/>
       </c>
       <c r="R12" t="str">
-        <f>IF(AE12&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE12:AF12) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="2"/>
+        <f>"#  " &amp; T12 &amp; U12 &amp; V12 &amp; " " &amp; W12 &amp; X12 &amp; Y12 &amp; " " &amp; Z12 &amp; AA12 &amp; AB12 &amp; " " &amp; AC12 &amp; AD12 &amp; AE12</f>
         <v>#  011 000 000 000</v>
       </c>
       <c r="T12">
@@ -1677,37 +1762,37 @@
         <v>0</v>
       </c>
       <c r="AF12" s="2">
-        <v>1.1538461538461537</v>
+        <v>1.0909090909090908</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T12:AE12,"&gt;0")</f>
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[8] == P[8], 0.909090909090909 / len(n_gram[i]), #  001 000 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C13 &amp; "] == P[" &amp; C13 &amp; "], " &amp; AF13 &amp; " / len(n_gram[i]), " &amp; S13</f>
+        <v>If(G[i] &amp; P[8] == P[8], 0.689655172413793 / len(n_gram[i]), #  000 000 000 100</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[8] == 512) #  001 000 000 000</v>
+        <f>"s.add(P[" &amp; C13 &amp; "] == " &amp; D13 &amp; ") " &amp; S13</f>
+        <v>s.add(P[8] == 4) #  000 000 000 100</v>
       </c>
       <c r="C13">
-        <f t="shared" si="6"/>
+        <f>C12+1</f>
         <v>8</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="7"/>
-        <v>512</v>
+        <f>T13*$T$1+U13*$U$1+V13*$V$1+W13*$W$1+X13*$X$1+Y13*$Y$1+Z13*$Z$1+AA13*$AA$1+AB13*$AB$1+AC13*$AC$1+AD13*$AD$1+AE13</f>
+        <v>4</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(9, 9, b.G[i]) == 1,  0.909090909090909 / len(n.grams[i]), #  001 000 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(2, 2, b.G[i]) == 1,  0.689655172413793 / len(n.grams[i]), #  000 000 000 100</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(9, 9, b.G[i]) == 1</v>
+        <f>G13 &amp; H13 &amp; I13 &amp; J13 &amp; K13 &amp; L13 &amp; M13 &amp; N13 &amp; O13 &amp; P13 &amp; Q13 &amp; R13</f>
+        <v>Extract(2, 2, b.G[i]) == 1</v>
       </c>
       <c r="G13" t="str">
         <f>IF(T13&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U13:$AE13) &gt; 0,", ",""), "")</f>
@@ -1719,7 +1804,7 @@
       </c>
       <c r="I13" t="str">
         <f>IF(V13&gt;0,"Extract(" &amp; V$2 &amp; ", " &amp; V$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(W13:$AE13) &gt; 0,", ",""), "")</f>
-        <v>Extract(9, 9, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="J13" t="str">
         <f>IF(W13&gt;0,"Extract(" &amp; W$2 &amp; ", " &amp; W$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(X13:$AE13) &gt; 0,", ",""), "")</f>
@@ -1747,19 +1832,19 @@
       </c>
       <c r="P13" t="str">
         <f>IF(AC13&gt;0,"Extract(" &amp; AC$2 &amp; ", " &amp; AC$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AD13:$AE13) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(2, 2, b.G[i]) == 1</v>
       </c>
       <c r="Q13" t="str">
         <f>IF(AD13&gt;0,"Extract(" &amp; AD$2 &amp; ", " &amp; AD$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AE13:$AE13) &gt; 0,", ",""), "")</f>
         <v/>
       </c>
       <c r="R13" t="str">
-        <f>IF(AE13&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE13:AF13) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S13" t="str">
-        <f t="shared" si="2"/>
-        <v>#  001 000 000 000</v>
+        <f>"#  " &amp; T13 &amp; U13 &amp; V13 &amp; " " &amp; W13 &amp; X13 &amp; Y13 &amp; " " &amp; Z13 &amp; AA13 &amp; AB13 &amp; " " &amp; AC13 &amp; AD13 &amp; AE13</f>
+        <v>#  000 000 000 100</v>
       </c>
       <c r="T13">
         <v>0</v>
@@ -1768,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -1789,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="AC13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD13">
         <v>0</v>
@@ -1798,41 +1883,41 @@
         <v>0</v>
       </c>
       <c r="AF13" s="2">
-        <v>0.90909090909090906</v>
+        <v>0.68965517241379315</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T13:AE13,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[9] == P[9], 0.8 / len(n_gram[i]), #  100 000 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C14 &amp; "] == P[" &amp; C14 &amp; "], " &amp; AF14 &amp; " / len(n_gram[i]), " &amp; S14</f>
+        <v>If(G[i] &amp; P[9] == P[9], 0.674157303370786 / len(n_gram[i]), #  000 000 100 000</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[9] == 2048) #  100 000 000 000</v>
+        <f>"s.add(P[" &amp; C14 &amp; "] == " &amp; D14 &amp; ") " &amp; S14</f>
+        <v>s.add(P[9] == 32) #  000 000 100 000</v>
       </c>
       <c r="C14">
-        <f t="shared" si="6"/>
+        <f>C13+1</f>
         <v>9</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="7"/>
-        <v>2048</v>
+        <f>T14*$T$1+U14*$U$1+V14*$V$1+W14*$W$1+X14*$X$1+Y14*$Y$1+Z14*$Z$1+AA14*$AA$1+AB14*$AB$1+AC14*$AC$1+AD14*$AD$1+AE14</f>
+        <v>32</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(11, 11, b.G[i]) == 1,  0.8 / len(n.grams[i]), #  100 000 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(5, 5, b.G[i]) == 1,  0.674157303370786 / len(n.grams[i]), #  000 000 100 000</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(11, 11, b.G[i]) == 1</v>
+        <f>G14 &amp; H14 &amp; I14 &amp; J14 &amp; K14 &amp; L14 &amp; M14 &amp; N14 &amp; O14 &amp; P14 &amp; Q14 &amp; R14</f>
+        <v>Extract(5, 5, b.G[i]) == 1</v>
       </c>
       <c r="G14" t="str">
         <f>IF(T14&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U14:$AE14) &gt; 0,", ",""), "")</f>
-        <v>Extract(11, 11, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="H14" t="str">
         <f>IF(U14&gt;0,"Extract(" &amp; U$2 &amp; ", " &amp; U$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(V14:$AE14) &gt; 0,", ",""), "")</f>
@@ -1856,7 +1941,7 @@
       </c>
       <c r="M14" t="str">
         <f>IF(Z14&gt;0,"Extract(" &amp; Z$2 &amp; ", " &amp; Z$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AA14:$AE14) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(5, 5, b.G[i]) == 1</v>
       </c>
       <c r="N14" t="str">
         <f>IF(AA14&gt;0,"Extract(" &amp; AA$2 &amp; ", " &amp; AA$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AB14:$AE14) &gt; 0,", ",""), "")</f>
@@ -1875,15 +1960,15 @@
         <v/>
       </c>
       <c r="R14" t="str">
-        <f>IF(AE14&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE14:AF14) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S14" t="str">
-        <f t="shared" si="2"/>
-        <v>#  100 000 000 000</v>
+        <f>"#  " &amp; T14 &amp; U14 &amp; V14 &amp; " " &amp; W14 &amp; X14 &amp; Y14 &amp; " " &amp; Z14 &amp; AA14 &amp; AB14 &amp; " " &amp; AC14 &amp; AD14 &amp; AE14</f>
+        <v>#  000 000 100 000</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -1901,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14">
         <v>0</v>
@@ -1919,37 +2004,37 @@
         <v>0</v>
       </c>
       <c r="AF14" s="2">
-        <v>0.8</v>
+        <v>0.6741573033707865</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T14:AE14,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[10] == P[10], 0.789473684210526 / len(n_gram[i]), #  000 000 000 100</v>
+        <f>"If(G[i] &amp; P[" &amp; C15 &amp; "] == P[" &amp; C15 &amp; "], " &amp; AF15 &amp; " / len(n_gram[i]), " &amp; S15</f>
+        <v>If(G[i] &amp; P[10] == P[10], 0.625 / len(n_gram[i]), #  000 000 000 001</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[10] == 4) #  000 000 000 100</v>
+        <f>"s.add(P[" &amp; C15 &amp; "] == " &amp; D15 &amp; ") " &amp; S15</f>
+        <v>s.add(P[10] == 1) #  000 000 000 001</v>
       </c>
       <c r="C15">
-        <f t="shared" si="6"/>
+        <f>C14+1</f>
         <v>10</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="7"/>
-        <v>4</v>
+        <f>T15*$T$1+U15*$U$1+V15*$V$1+W15*$W$1+X15*$X$1+Y15*$Y$1+Z15*$Z$1+AA15*$AA$1+AB15*$AB$1+AC15*$AC$1+AD15*$AD$1+AE15</f>
+        <v>1</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(2, 2, b.G[i]) == 1,  0.789473684210526 / len(n.grams[i]), #  000 000 000 100</v>
+        <f>"If(" &amp; IF(SUM(T15:AE15) &gt; 1, "And(" &amp; F15 &amp; ")", F15) &amp; ",  " &amp; AF15 &amp; " / len(n.grams[i]), " &amp; S15</f>
+        <v>If(Extract(0, 0, b.G[i]) == 1,  0.625 / len(n.grams[i]), #  000 000 000 001</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(2, 2, b.G[i]) == 1</v>
+        <f>G15 &amp; H15 &amp; I15 &amp; J15 &amp; K15 &amp; L15 &amp; M15 &amp; N15 &amp; O15 &amp; P15 &amp; Q15 &amp; R15</f>
+        <v>Extract(0, 0, b.G[i]) == 1</v>
       </c>
       <c r="G15" t="str">
         <f>IF(T15&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U15:$AE15) &gt; 0,", ",""), "")</f>
@@ -1989,19 +2074,19 @@
       </c>
       <c r="P15" t="str">
         <f>IF(AC15&gt;0,"Extract(" &amp; AC$2 &amp; ", " &amp; AC$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AD15:$AE15) &gt; 0,", ",""), "")</f>
-        <v>Extract(2, 2, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="Q15" t="str">
         <f>IF(AD15&gt;0,"Extract(" &amp; AD$2 &amp; ", " &amp; AD$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AE15:$AE15) &gt; 0,", ",""), "")</f>
         <v/>
       </c>
       <c r="R15" t="str">
-        <f>IF(AE15&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE15:AF15) &gt; 0,", ",""), "")</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>Extract(0, 0, b.G[i]) == 1</v>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 000 000 100</v>
+        <f>"#  " &amp; T15 &amp; U15 &amp; V15 &amp; " " &amp; W15 &amp; X15 &amp; Y15 &amp; " " &amp; Z15 &amp; AA15 &amp; AB15 &amp; " " &amp; AC15 &amp; AD15 &amp; AE15</f>
+        <v>#  000 000 000 001</v>
       </c>
       <c r="T15">
         <v>0</v>
@@ -2031,46 +2116,46 @@
         <v>0</v>
       </c>
       <c r="AC15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD15">
         <v>0</v>
       </c>
       <c r="AE15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15" s="2">
-        <v>0.78947368421052633</v>
+        <v>0.625</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T15:AE15,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[11] == P[11], 0.789473684210526 / len(n_gram[i]), #  000 000 000 001</v>
+        <f>"If(G[i] &amp; P[" &amp; C16 &amp; "] == P[" &amp; C16 &amp; "], " &amp; AF16 &amp; " / len(n_gram[i]), " &amp; S16</f>
+        <v>If(G[i] &amp; P[11] == P[11], 0.594059405940594 / len(n_gram[i]), #  000 000 001 000</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[11] == 1) #  000 000 000 001</v>
+        <f>"s.add(P[" &amp; C16 &amp; "] == " &amp; D16 &amp; ") " &amp; S16</f>
+        <v>s.add(P[11] == 8) #  000 000 001 000</v>
       </c>
       <c r="C16">
-        <f t="shared" si="6"/>
+        <f>C15+1</f>
         <v>11</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>T16*$T$1+U16*$U$1+V16*$V$1+W16*$W$1+X16*$X$1+Y16*$Y$1+Z16*$Z$1+AA16*$AA$1+AB16*$AB$1+AC16*$AC$1+AD16*$AD$1+AE16</f>
+        <v>8</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(0, 0, b.G[i]) == 1, ,  0.789473684210526 / len(n.grams[i]), #  000 000 000 001</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(3, 3, b.G[i]) == 1,  0.594059405940594 / len(n.grams[i]), #  000 000 001 000</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">Extract(0, 0, b.G[i]) == 1, </v>
+        <f>G16 &amp; H16 &amp; I16 &amp; J16 &amp; K16 &amp; L16 &amp; M16 &amp; N16 &amp; O16 &amp; P16 &amp; Q16 &amp; R16</f>
+        <v>Extract(3, 3, b.G[i]) == 1</v>
       </c>
       <c r="G16" t="str">
         <f>IF(T16&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U16:$AE16) &gt; 0,", ",""), "")</f>
@@ -2106,7 +2191,7 @@
       </c>
       <c r="O16" t="str">
         <f>IF(AB16&gt;0,"Extract(" &amp; AB$2 &amp; ", " &amp; AB$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AC16:$AE16) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(3, 3, b.G[i]) == 1</v>
       </c>
       <c r="P16" t="str">
         <f>IF(AC16&gt;0,"Extract(" &amp; AC$2 &amp; ", " &amp; AC$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AD16:$AE16) &gt; 0,", ",""), "")</f>
@@ -2117,12 +2202,12 @@
         <v/>
       </c>
       <c r="R16" t="str">
-        <f>IF(AE16&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE16:AF16) &gt; 0,", ",""), "")</f>
-        <v xml:space="preserve">Extract(0, 0, b.G[i]) == 1, </v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 000 000 001</v>
+        <f>"#  " &amp; T16 &amp; U16 &amp; V16 &amp; " " &amp; W16 &amp; X16 &amp; Y16 &amp; " " &amp; Z16 &amp; AA16 &amp; AB16 &amp; " " &amp; AC16 &amp; AD16 &amp; AE16</f>
+        <v>#  000 000 001 000</v>
       </c>
       <c r="T16">
         <v>0</v>
@@ -2149,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="AB16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC16">
         <v>0</v>
@@ -2158,40 +2243,40 @@
         <v>0</v>
       </c>
       <c r="AE16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF16" s="2">
-        <v>0.78947368421052633</v>
+        <v>0.59405940594059403</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T16:AE16,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[12] == P[12], 0.779220779220779 / len(n_gram[i]), #  000 001 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C17 &amp; "] == P[" &amp; C17 &amp; "], " &amp; AF17 &amp; " / len(n_gram[i]), " &amp; S17</f>
+        <v>If(G[i] &amp; P[12] == P[12], 0.560747663551402 / len(n_gram[i]), #  001 000 000 000</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[12] == 64) #  000 001 000 000</v>
+        <f>"s.add(P[" &amp; C17 &amp; "] == " &amp; D17 &amp; ") " &amp; S17</f>
+        <v>s.add(P[12] == 512) #  001 000 000 000</v>
       </c>
       <c r="C17">
-        <f t="shared" si="6"/>
+        <f>C16+1</f>
         <v>12</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="7"/>
-        <v>64</v>
+        <f>T17*$T$1+U17*$U$1+V17*$V$1+W17*$W$1+X17*$X$1+Y17*$Y$1+Z17*$Z$1+AA17*$AA$1+AB17*$AB$1+AC17*$AC$1+AD17*$AD$1+AE17</f>
+        <v>512</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(6, 6, b.G[i]) == 1,  0.779220779220779 / len(n.grams[i]), #  000 001 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(9, 9, b.G[i]) == 1,  0.560747663551402 / len(n.grams[i]), #  001 000 000 000</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(6, 6, b.G[i]) == 1</v>
+        <f>G17 &amp; H17 &amp; I17 &amp; J17 &amp; K17 &amp; L17 &amp; M17 &amp; N17 &amp; O17 &amp; P17 &amp; Q17 &amp; R17</f>
+        <v>Extract(9, 9, b.G[i]) == 1</v>
       </c>
       <c r="G17" t="str">
         <f>IF(T17&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U17:$AE17) &gt; 0,", ",""), "")</f>
@@ -2203,7 +2288,7 @@
       </c>
       <c r="I17" t="str">
         <f>IF(V17&gt;0,"Extract(" &amp; V$2 &amp; ", " &amp; V$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(W17:$AE17) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(9, 9, b.G[i]) == 1</v>
       </c>
       <c r="J17" t="str">
         <f>IF(W17&gt;0,"Extract(" &amp; W$2 &amp; ", " &amp; W$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(X17:$AE17) &gt; 0,", ",""), "")</f>
@@ -2215,7 +2300,7 @@
       </c>
       <c r="L17" t="str">
         <f>IF(Y17&gt;0,"Extract(" &amp; Y$2 &amp; ", " &amp; Y$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Z17:$AE17) &gt; 0,", ",""), "")</f>
-        <v>Extract(6, 6, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="M17" t="str">
         <f>IF(Z17&gt;0,"Extract(" &amp; Z$2 &amp; ", " &amp; Z$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AA17:$AE17) &gt; 0,", ",""), "")</f>
@@ -2238,12 +2323,12 @@
         <v/>
       </c>
       <c r="R17" t="str">
-        <f>IF(AE17&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE17:AF17) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 001 000 000</v>
+        <f>"#  " &amp; T17 &amp; U17 &amp; V17 &amp; " " &amp; W17 &amp; X17 &amp; Y17 &amp; " " &amp; Z17 &amp; AA17 &amp; AB17 &amp; " " &amp; AC17 &amp; AD17 &amp; AE17</f>
+        <v>#  001 000 000 000</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -2252,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17">
         <v>0</v>
@@ -2261,7 +2346,7 @@
         <v>0</v>
       </c>
       <c r="Y17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17">
         <v>0</v>
@@ -2282,37 +2367,37 @@
         <v>0</v>
       </c>
       <c r="AF17" s="2">
-        <v>0.77922077922077926</v>
+        <v>0.56074766355140182</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T17:AE17,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[13] == P[13], 0.769230769230769 / len(n_gram[i]), #  000 000 001 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C18 &amp; "] == P[" &amp; C18 &amp; "], " &amp; AF18 &amp; " / len(n_gram[i]), " &amp; S18</f>
+        <v>If(G[i] &amp; P[13] == P[13], 0.538116591928251 / len(n_gram[i]), #  000 000 000 010</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[13] == 8) #  000 000 001 000</v>
+        <f>"s.add(P[" &amp; C18 &amp; "] == " &amp; D18 &amp; ") " &amp; S18</f>
+        <v>s.add(P[13] == 2) #  000 000 000 010</v>
       </c>
       <c r="C18">
-        <f t="shared" si="6"/>
+        <f>C17+1</f>
         <v>13</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="7"/>
-        <v>8</v>
+        <f>T18*$T$1+U18*$U$1+V18*$V$1+W18*$W$1+X18*$X$1+Y18*$Y$1+Z18*$Z$1+AA18*$AA$1+AB18*$AB$1+AC18*$AC$1+AD18*$AD$1+AE18</f>
+        <v>2</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(3, 3, b.G[i]) == 1,  0.769230769230769 / len(n.grams[i]), #  000 000 001 000</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(1, 1, b.G[i]) == 1,  0.538116591928251 / len(n.grams[i]), #  000 000 000 010</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(3, 3, b.G[i]) == 1</v>
+        <f>G18 &amp; H18 &amp; I18 &amp; J18 &amp; K18 &amp; L18 &amp; M18 &amp; N18 &amp; O18 &amp; P18 &amp; Q18 &amp; R18</f>
+        <v>Extract(1, 1, b.G[i]) == 1</v>
       </c>
       <c r="G18" t="str">
         <f>IF(T18&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U18:$AE18) &gt; 0,", ",""), "")</f>
@@ -2348,7 +2433,7 @@
       </c>
       <c r="O18" t="str">
         <f>IF(AB18&gt;0,"Extract(" &amp; AB$2 &amp; ", " &amp; AB$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AC18:$AE18) &gt; 0,", ",""), "")</f>
-        <v>Extract(3, 3, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="P18" t="str">
         <f>IF(AC18&gt;0,"Extract(" &amp; AC$2 &amp; ", " &amp; AC$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AD18:$AE18) &gt; 0,", ",""), "")</f>
@@ -2356,15 +2441,15 @@
       </c>
       <c r="Q18" t="str">
         <f>IF(AD18&gt;0,"Extract(" &amp; AD$2 &amp; ", " &amp; AD$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AE18:$AE18) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(1, 1, b.G[i]) == 1</v>
       </c>
       <c r="R18" t="str">
-        <f>IF(AE18&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE18:AF18) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 000 001 000</v>
+        <f>"#  " &amp; T18 &amp; U18 &amp; V18 &amp; " " &amp; W18 &amp; X18 &amp; Y18 &amp; " " &amp; Z18 &amp; AA18 &amp; AB18 &amp; " " &amp; AC18 &amp; AD18 &amp; AE18</f>
+        <v>#  000 000 000 010</v>
       </c>
       <c r="T18">
         <v>0</v>
@@ -2391,53 +2476,53 @@
         <v>0</v>
       </c>
       <c r="AB18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18">
         <v>0</v>
       </c>
       <c r="AD18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE18">
         <v>0</v>
       </c>
       <c r="AF18" s="2">
-        <v>0.76923076923076927</v>
+        <v>0.53811659192825112</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T18:AE18,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[14] == P[14], 0.75 / len(n_gram[i]), #  000 100 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C19 &amp; "] == P[" &amp; C19 &amp; "], " &amp; AF19 &amp; " / len(n_gram[i]), " &amp; S19</f>
+        <v>If(G[i] &amp; P[14] == P[14], 0.530973451327434 / len(n_gram[i]), #  100 000 000 000</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[14] == 256) #  000 100 000 000</v>
+        <f>"s.add(P[" &amp; C19 &amp; "] == " &amp; D19 &amp; ") " &amp; S19</f>
+        <v>s.add(P[14] == 2048) #  100 000 000 000</v>
       </c>
       <c r="C19">
-        <f t="shared" si="6"/>
+        <f>C18+1</f>
         <v>14</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="7"/>
-        <v>256</v>
+        <f>T19*$T$1+U19*$U$1+V19*$V$1+W19*$W$1+X19*$X$1+Y19*$Y$1+Z19*$Z$1+AA19*$AA$1+AB19*$AB$1+AC19*$AC$1+AD19*$AD$1+AE19</f>
+        <v>2048</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(8, 8, b.G[i]) == 1,  0.75 / len(n.grams[i]), #  000 100 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(11, 11, b.G[i]) == 1,  0.530973451327434 / len(n.grams[i]), #  100 000 000 000</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(8, 8, b.G[i]) == 1</v>
+        <f>G19 &amp; H19 &amp; I19 &amp; J19 &amp; K19 &amp; L19 &amp; M19 &amp; N19 &amp; O19 &amp; P19 &amp; Q19 &amp; R19</f>
+        <v>Extract(11, 11, b.G[i]) == 1</v>
       </c>
       <c r="G19" t="str">
         <f>IF(T19&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U19:$AE19) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(11, 11, b.G[i]) == 1</v>
       </c>
       <c r="H19" t="str">
         <f>IF(U19&gt;0,"Extract(" &amp; U$2 &amp; ", " &amp; U$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(V19:$AE19) &gt; 0,", ",""), "")</f>
@@ -2449,7 +2534,7 @@
       </c>
       <c r="J19" t="str">
         <f>IF(W19&gt;0,"Extract(" &amp; W$2 &amp; ", " &amp; W$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(X19:$AE19) &gt; 0,", ",""), "")</f>
-        <v>Extract(8, 8, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="K19" t="str">
         <f>IF(X19&gt;0,"Extract(" &amp; X$2 &amp; ", " &amp; X$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Y19:$AE19) &gt; 0,", ",""), "")</f>
@@ -2480,15 +2565,15 @@
         <v/>
       </c>
       <c r="R19" t="str">
-        <f>IF(AE19&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE19:AF19) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 100 000 000</v>
+        <f>"#  " &amp; T19 &amp; U19 &amp; V19 &amp; " " &amp; W19 &amp; X19 &amp; Y19 &amp; " " &amp; Z19 &amp; AA19 &amp; AB19 &amp; " " &amp; AC19 &amp; AD19 &amp; AE19</f>
+        <v>#  100 000 000 000</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -2497,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X19">
         <v>0</v>
@@ -2524,37 +2609,37 @@
         <v>0</v>
       </c>
       <c r="AF19" s="2">
-        <v>0.75</v>
+        <v>0.53097345132743368</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T19:AE19,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[15] == P[15], 0.731707317073171 / len(n_gram[i]), #  000 000 100 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C20 &amp; "] == P[" &amp; C20 &amp; "], " &amp; AF20 &amp; " / len(n_gram[i]), " &amp; S20</f>
+        <v>If(G[i] &amp; P[15] == P[15], 0.530973451327434 / len(n_gram[i]), #  000 100 000 000</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[15] == 32) #  000 000 100 000</v>
+        <f>"s.add(P[" &amp; C20 &amp; "] == " &amp; D20 &amp; ") " &amp; S20</f>
+        <v>s.add(P[15] == 256) #  000 100 000 000</v>
       </c>
       <c r="C20">
-        <f t="shared" si="6"/>
+        <f>C19+1</f>
         <v>15</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="7"/>
-        <v>32</v>
+        <f>T20*$T$1+U20*$U$1+V20*$V$1+W20*$W$1+X20*$X$1+Y20*$Y$1+Z20*$Z$1+AA20*$AA$1+AB20*$AB$1+AC20*$AC$1+AD20*$AD$1+AE20</f>
+        <v>256</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(5, 5, b.G[i]) == 1,  0.731707317073171 / len(n.grams[i]), #  000 000 100 000</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(8, 8, b.G[i]) == 1,  0.530973451327434 / len(n.grams[i]), #  000 100 000 000</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(5, 5, b.G[i]) == 1</v>
+        <f>G20 &amp; H20 &amp; I20 &amp; J20 &amp; K20 &amp; L20 &amp; M20 &amp; N20 &amp; O20 &amp; P20 &amp; Q20 &amp; R20</f>
+        <v>Extract(8, 8, b.G[i]) == 1</v>
       </c>
       <c r="G20" t="str">
         <f>IF(T20&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U20:$AE20) &gt; 0,", ",""), "")</f>
@@ -2570,7 +2655,7 @@
       </c>
       <c r="J20" t="str">
         <f>IF(W20&gt;0,"Extract(" &amp; W$2 &amp; ", " &amp; W$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(X20:$AE20) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(8, 8, b.G[i]) == 1</v>
       </c>
       <c r="K20" t="str">
         <f>IF(X20&gt;0,"Extract(" &amp; X$2 &amp; ", " &amp; X$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Y20:$AE20) &gt; 0,", ",""), "")</f>
@@ -2582,7 +2667,7 @@
       </c>
       <c r="M20" t="str">
         <f>IF(Z20&gt;0,"Extract(" &amp; Z$2 &amp; ", " &amp; Z$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AA20:$AE20) &gt; 0,", ",""), "")</f>
-        <v>Extract(5, 5, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="N20" t="str">
         <f>IF(AA20&gt;0,"Extract(" &amp; AA$2 &amp; ", " &amp; AA$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AB20:$AE20) &gt; 0,", ",""), "")</f>
@@ -2601,12 +2686,12 @@
         <v/>
       </c>
       <c r="R20" t="str">
-        <f>IF(AE20&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE20:AF20) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 000 100 000</v>
+        <f>"#  " &amp; T20 &amp; U20 &amp; V20 &amp; " " &amp; W20 &amp; X20 &amp; Y20 &amp; " " &amp; Z20 &amp; AA20 &amp; AB20 &amp; " " &amp; AC20 &amp; AD20 &amp; AE20</f>
+        <v>#  000 100 000 000</v>
       </c>
       <c r="T20">
         <v>0</v>
@@ -2618,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="W20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -2627,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="Z20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA20">
         <v>0</v>
@@ -2645,37 +2730,37 @@
         <v>0</v>
       </c>
       <c r="AF20" s="2">
-        <v>0.73170731707317072</v>
+        <v>0.53097345132743368</v>
       </c>
       <c r="AG20">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T20:AE20,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[16] == P[16], 0.621761658031088 / len(n_gram[i]), #  000 000 000 010</v>
+        <f>"If(G[i] &amp; P[" &amp; C21 &amp; "] == P[" &amp; C21 &amp; "], " &amp; AF21 &amp; " / len(n_gram[i]), " &amp; S21</f>
+        <v>If(G[i] &amp; P[16] == P[16], 0.521739130434783 / len(n_gram[i]), #  000 001 000 000</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[16] == 2) #  000 000 000 010</v>
+        <f>"s.add(P[" &amp; C21 &amp; "] == " &amp; D21 &amp; ") " &amp; S21</f>
+        <v>s.add(P[16] == 64) #  000 001 000 000</v>
       </c>
       <c r="C21">
-        <f t="shared" si="6"/>
+        <f>C20+1</f>
         <v>16</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f>T21*$T$1+U21*$U$1+V21*$V$1+W21*$W$1+X21*$X$1+Y21*$Y$1+Z21*$Z$1+AA21*$AA$1+AB21*$AB$1+AC21*$AC$1+AD21*$AD$1+AE21</f>
+        <v>64</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(1, 1, b.G[i]) == 1,  0.621761658031088 / len(n.grams[i]), #  000 000 000 010</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(6, 6, b.G[i]) == 1,  0.521739130434783 / len(n.grams[i]), #  000 001 000 000</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(1, 1, b.G[i]) == 1</v>
+        <f>G21 &amp; H21 &amp; I21 &amp; J21 &amp; K21 &amp; L21 &amp; M21 &amp; N21 &amp; O21 &amp; P21 &amp; Q21 &amp; R21</f>
+        <v>Extract(6, 6, b.G[i]) == 1</v>
       </c>
       <c r="G21" t="str">
         <f>IF(T21&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U21:$AE21) &gt; 0,", ",""), "")</f>
@@ -2699,7 +2784,7 @@
       </c>
       <c r="L21" t="str">
         <f>IF(Y21&gt;0,"Extract(" &amp; Y$2 &amp; ", " &amp; Y$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Z21:$AE21) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(6, 6, b.G[i]) == 1</v>
       </c>
       <c r="M21" t="str">
         <f>IF(Z21&gt;0,"Extract(" &amp; Z$2 &amp; ", " &amp; Z$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AA21:$AE21) &gt; 0,", ",""), "")</f>
@@ -2719,15 +2804,15 @@
       </c>
       <c r="Q21" t="str">
         <f>IF(AD21&gt;0,"Extract(" &amp; AD$2 &amp; ", " &amp; AD$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AE21:$AE21) &gt; 0,", ",""), "")</f>
-        <v>Extract(1, 1, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="R21" t="str">
-        <f>IF(AE21&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE21:AF21) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 000 000 010</v>
+        <f>"#  " &amp; T21 &amp; U21 &amp; V21 &amp; " " &amp; W21 &amp; X21 &amp; Y21 &amp; " " &amp; Z21 &amp; AA21 &amp; AB21 &amp; " " &amp; AC21 &amp; AD21 &amp; AE21</f>
+        <v>#  000 001 000 000</v>
       </c>
       <c r="T21">
         <v>0</v>
@@ -2745,7 +2830,7 @@
         <v>0</v>
       </c>
       <c r="Y21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21">
         <v>0</v>
@@ -2760,43 +2845,43 @@
         <v>0</v>
       </c>
       <c r="AD21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE21">
         <v>0</v>
       </c>
       <c r="AF21" s="2">
-        <v>0.62176165803108807</v>
+        <v>0.52173913043478259</v>
       </c>
       <c r="AG21">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T21:AE21,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[17] == P[17], 0.542986425339366 / len(n_gram[i]), #  000 000 010 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C22 &amp; "] == P[" &amp; C22 &amp; "], " &amp; AF22 &amp; " / len(n_gram[i]), " &amp; S22</f>
+        <v>If(G[i] &amp; P[17] == P[17], 0.470588235294118 / len(n_gram[i]), #  000 010 000 000</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[17] == 16) #  000 000 010 000</v>
+        <f>"s.add(P[" &amp; C22 &amp; "] == " &amp; D22 &amp; ") " &amp; S22</f>
+        <v>s.add(P[17] == 128) #  000 010 000 000</v>
       </c>
       <c r="C22">
-        <f t="shared" si="6"/>
+        <f>C21+1</f>
         <v>17</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="7"/>
-        <v>16</v>
+        <f>T22*$T$1+U22*$U$1+V22*$V$1+W22*$W$1+X22*$X$1+Y22*$Y$1+Z22*$Z$1+AA22*$AA$1+AB22*$AB$1+AC22*$AC$1+AD22*$AD$1+AE22</f>
+        <v>128</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(4, 4, b.G[i]) == 1,  0.542986425339366 / len(n.grams[i]), #  000 000 010 000</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(7, 7, b.G[i]) == 1,  0.470588235294118 / len(n.grams[i]), #  000 010 000 000</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(4, 4, b.G[i]) == 1</v>
+        <f>G22 &amp; H22 &amp; I22 &amp; J22 &amp; K22 &amp; L22 &amp; M22 &amp; N22 &amp; O22 &amp; P22 &amp; Q22 &amp; R22</f>
+        <v>Extract(7, 7, b.G[i]) == 1</v>
       </c>
       <c r="G22" t="str">
         <f>IF(T22&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U22:$AE22) &gt; 0,", ",""), "")</f>
@@ -2816,7 +2901,7 @@
       </c>
       <c r="K22" t="str">
         <f>IF(X22&gt;0,"Extract(" &amp; X$2 &amp; ", " &amp; X$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Y22:$AE22) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(7, 7, b.G[i]) == 1</v>
       </c>
       <c r="L22" t="str">
         <f>IF(Y22&gt;0,"Extract(" &amp; Y$2 &amp; ", " &amp; Y$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Z22:$AE22) &gt; 0,", ",""), "")</f>
@@ -2828,7 +2913,7 @@
       </c>
       <c r="N22" t="str">
         <f>IF(AA22&gt;0,"Extract(" &amp; AA$2 &amp; ", " &amp; AA$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AB22:$AE22) &gt; 0,", ",""), "")</f>
-        <v>Extract(4, 4, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="O22" t="str">
         <f>IF(AB22&gt;0,"Extract(" &amp; AB$2 &amp; ", " &amp; AB$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AC22:$AE22) &gt; 0,", ",""), "")</f>
@@ -2843,12 +2928,12 @@
         <v/>
       </c>
       <c r="R22" t="str">
-        <f>IF(AE22&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE22:AF22) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 000 010 000</v>
+        <f>"#  " &amp; T22 &amp; U22 &amp; V22 &amp; " " &amp; W22 &amp; X22 &amp; Y22 &amp; " " &amp; Z22 &amp; AA22 &amp; AB22 &amp; " " &amp; AC22 &amp; AD22 &amp; AE22</f>
+        <v>#  000 010 000 000</v>
       </c>
       <c r="T22">
         <v>0</v>
@@ -2863,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="X22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y22">
         <v>0</v>
@@ -2872,7 +2957,7 @@
         <v>0</v>
       </c>
       <c r="AA22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB22">
         <v>0</v>
@@ -2887,37 +2972,37 @@
         <v>0</v>
       </c>
       <c r="AF22" s="2">
-        <v>0.54298642533936647</v>
+        <v>0.47058823529411764</v>
       </c>
       <c r="AG22">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T22:AE22,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[18] == P[18], 0.49792531120332 / len(n_gram[i]), #  000 010 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C23 &amp; "] == P[" &amp; C23 &amp; "], " &amp; AF23 &amp; " / len(n_gram[i]), " &amp; S23</f>
+        <v>If(G[i] &amp; P[18] == P[18], 0.465116279069767 / len(n_gram[i]), #  000 000 010 000</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="5"/>
-        <v>s.add(P[18] == 128) #  000 010 000 000</v>
+        <f>"s.add(P[" &amp; C23 &amp; "] == " &amp; D23 &amp; ") " &amp; S23</f>
+        <v>s.add(P[18] == 16) #  000 000 010 000</v>
       </c>
       <c r="C23">
-        <f t="shared" si="6"/>
+        <f>C22+1</f>
         <v>18</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="7"/>
-        <v>128</v>
+        <f>T23*$T$1+U23*$U$1+V23*$V$1+W23*$W$1+X23*$X$1+Y23*$Y$1+Z23*$Z$1+AA23*$AA$1+AB23*$AB$1+AC23*$AC$1+AD23*$AD$1+AE23</f>
+        <v>16</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(7, 7, b.G[i]) == 1,  0.49792531120332 / len(n.grams[i]), #  000 010 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(4, 4, b.G[i]) == 1,  0.465116279069767 / len(n.grams[i]), #  000 000 010 000</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="1"/>
-        <v>Extract(7, 7, b.G[i]) == 1</v>
+        <f>G23 &amp; H23 &amp; I23 &amp; J23 &amp; K23 &amp; L23 &amp; M23 &amp; N23 &amp; O23 &amp; P23 &amp; Q23 &amp; R23</f>
+        <v>Extract(4, 4, b.G[i]) == 1</v>
       </c>
       <c r="G23" t="str">
         <f>IF(T23&gt;0,"Extract(" &amp; T$2 &amp; ", " &amp; T$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(U23:$AE23) &gt; 0,", ",""), "")</f>
@@ -2937,7 +3022,7 @@
       </c>
       <c r="K23" t="str">
         <f>IF(X23&gt;0,"Extract(" &amp; X$2 &amp; ", " &amp; X$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Y23:$AE23) &gt; 0,", ",""), "")</f>
-        <v>Extract(7, 7, b.G[i]) == 1</v>
+        <v/>
       </c>
       <c r="L23" t="str">
         <f>IF(Y23&gt;0,"Extract(" &amp; Y$2 &amp; ", " &amp; Y$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(Z23:$AE23) &gt; 0,", ",""), "")</f>
@@ -2949,7 +3034,7 @@
       </c>
       <c r="N23" t="str">
         <f>IF(AA23&gt;0,"Extract(" &amp; AA$2 &amp; ", " &amp; AA$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AB23:$AE23) &gt; 0,", ",""), "")</f>
-        <v/>
+        <v>Extract(4, 4, b.G[i]) == 1</v>
       </c>
       <c r="O23" t="str">
         <f>IF(AB23&gt;0,"Extract(" &amp; AB$2 &amp; ", " &amp; AB$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM(AC23:$AE23) &gt; 0,", ",""), "")</f>
@@ -2964,12 +3049,12 @@
         <v/>
       </c>
       <c r="R23" t="str">
-        <f>IF(AE23&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE23:AF23) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="2"/>
-        <v>#  000 010 000 000</v>
+        <f>"#  " &amp; T23 &amp; U23 &amp; V23 &amp; " " &amp; W23 &amp; X23 &amp; Y23 &amp; " " &amp; Z23 &amp; AA23 &amp; AB23 &amp; " " &amp; AC23 &amp; AD23 &amp; AE23</f>
+        <v>#  000 000 010 000</v>
       </c>
       <c r="T23">
         <v>0</v>
@@ -2984,7 +3069,7 @@
         <v>0</v>
       </c>
       <c r="X23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23">
         <v>0</v>
@@ -2993,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="AA23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB23">
         <v>0</v>
@@ -3008,36 +3093,36 @@
         <v>0</v>
       </c>
       <c r="AF23" s="2">
-        <v>0.49792531120331951</v>
+        <v>0.46511627906976744</v>
       </c>
       <c r="AG23">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T23:AE23,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f t="shared" si="4"/>
-        <v>If(G[i] &amp; P[19] == P[19], 0.47244094488189 / len(n_gram[i]), #  010 000 000 000</v>
+        <f>"If(G[i] &amp; P[" &amp; C24 &amp; "] == P[" &amp; C24 &amp; "], " &amp; AF24 &amp; " / len(n_gram[i]), " &amp; S24</f>
+        <v>If(G[i] &amp; P[19] == P[19], 0.452830188679245 / len(n_gram[i]), #  010 000 000 000</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="5"/>
+        <f>"s.add(P[" &amp; C24 &amp; "] == " &amp; D24 &amp; ") " &amp; S24</f>
         <v>s.add(P[19] == 1024) #  010 000 000 000</v>
       </c>
       <c r="C24">
-        <f t="shared" si="6"/>
+        <f>C23+1</f>
         <v>19</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="7"/>
+        <f>T24*$T$1+U24*$U$1+V24*$V$1+W24*$W$1+X24*$X$1+Y24*$Y$1+Z24*$Z$1+AA24*$AA$1+AB24*$AB$1+AC24*$AC$1+AD24*$AD$1+AE24</f>
         <v>1024</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="8"/>
-        <v>If(Extract(10, 10, b.G[i]) == 1,  0.47244094488189 / len(n.grams[i]), #  010 000 000 000</v>
+        <f t="shared" si="1"/>
+        <v>If(Extract(10, 10, b.G[i]) == 1,  0.452830188679245 / len(n.grams[i]), #  010 000 000 000</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="1"/>
+        <f>G24 &amp; H24 &amp; I24 &amp; J24 &amp; K24 &amp; L24 &amp; M24 &amp; N24 &amp; O24 &amp; P24 &amp; Q24 &amp; R24</f>
         <v>Extract(10, 10, b.G[i]) == 1</v>
       </c>
       <c r="G24" t="str">
@@ -3085,11 +3170,11 @@
         <v/>
       </c>
       <c r="R24" t="str">
-        <f>IF(AE24&gt;0,"Extract(" &amp; AE$2 &amp; ", " &amp; AE$2 &amp; ", b.G[i]) == 1" &amp; IF(SUM($AE24:AF24) &gt; 0,", ",""), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="2"/>
+        <f>"#  " &amp; T24 &amp; U24 &amp; V24 &amp; " " &amp; W24 &amp; X24 &amp; Y24 &amp; " " &amp; Z24 &amp; AA24 &amp; AB24 &amp; " " &amp; AC24 &amp; AD24 &amp; AE24</f>
         <v>#  010 000 000 000</v>
       </c>
       <c r="T24">
@@ -3129,15 +3214,15 @@
         <v>0</v>
       </c>
       <c r="AF24" s="2">
-        <v>0.47244094488188976</v>
+        <v>0.45283018867924529</v>
       </c>
       <c r="AG24">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(T24:AE24,"&gt;0")</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="T5:AG24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:AG24">
     <sortCondition descending="1" ref="AG5:AG24"/>
     <sortCondition descending="1" ref="AF5:AF24"/>
   </sortState>
@@ -3158,19 +3243,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5145A5A3-896F-4F2D-9E96-594996D205F2}">
-  <dimension ref="A1:P38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5145A5A3-896F-4F2D-9E96-594996D205F2}">
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M4" sqref="A4:M23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="9.140625" style="6"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
@@ -3188,7 +3275,7 @@
       <c r="K1" s="11"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -3221,8 +3308,14 @@
       <c r="P2" s="8">
         <v>43974</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="13">
+        <v>44128</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3271,8 +3364,14 @@
       <c r="P3">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>60</v>
+      </c>
+      <c r="R3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -3310,15 +3409,23 @@
         <v>0</v>
       </c>
       <c r="M4" s="6">
-        <f>60/SUM(N4:P4)</f>
-        <v>0.47244094488188976</v>
+        <f>60/R4</f>
+        <v>0.45283018867924529</v>
       </c>
       <c r="N4" s="9">
         <f>254/2</f>
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <f>265/2</f>
+        <v>132.5</v>
+      </c>
+      <c r="R4">
+        <f>265/2</f>
+        <v>132.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -3356,15 +3463,23 @@
         <v>0</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" ref="M5:M23" si="0">60/SUM(N5:P5)</f>
-        <v>0.49792531120331951</v>
+        <f t="shared" ref="M5:M23" si="0">60/R5</f>
+        <v>0.47058823529411764</v>
       </c>
       <c r="N5">
         <f>241/2</f>
         <v>120.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <f>255/2</f>
+        <v>127.5</v>
+      </c>
+      <c r="R5">
+        <f>255/2</f>
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -3403,14 +3518,22 @@
       </c>
       <c r="M6" s="6">
         <f t="shared" si="0"/>
-        <v>0.54298642533936647</v>
+        <v>0.46511627906976744</v>
       </c>
       <c r="N6" s="9">
         <f>221/2</f>
         <v>110.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <f>258/2</f>
+        <v>129</v>
+      </c>
+      <c r="R6">
+        <f>258/2</f>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -3449,14 +3572,22 @@
       </c>
       <c r="M7" s="6">
         <f t="shared" si="0"/>
-        <v>0.62176165803108807</v>
+        <v>0.53811659192825112</v>
       </c>
       <c r="N7" s="9">
         <f>193/2</f>
         <v>96.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <f>223/2</f>
+        <v>111.5</v>
+      </c>
+      <c r="R7">
+        <f>223/2</f>
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3495,13 +3626,19 @@
       </c>
       <c r="M8" s="6">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.53097345132743368</v>
       </c>
       <c r="N8" s="9">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>113</v>
+      </c>
+      <c r="R8">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3540,13 +3677,19 @@
       </c>
       <c r="M9" s="6">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.53097345132743368</v>
       </c>
       <c r="N9" s="9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>113</v>
+      </c>
+      <c r="R9">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3585,13 +3728,19 @@
       </c>
       <c r="M10" s="6">
         <f t="shared" si="0"/>
-        <v>0.73170731707317072</v>
+        <v>0.6741573033707865</v>
       </c>
       <c r="N10" s="9">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>89</v>
+      </c>
+      <c r="R10">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3630,13 +3779,19 @@
       </c>
       <c r="M11" s="6">
         <f t="shared" si="0"/>
-        <v>0.78947368421052633</v>
+        <v>0.68965517241379315</v>
       </c>
       <c r="N11" s="9">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>87</v>
+      </c>
+      <c r="R11">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3675,13 +3830,19 @@
       </c>
       <c r="M12" s="6">
         <f t="shared" si="0"/>
-        <v>0.90909090909090906</v>
+        <v>0.56074766355140182</v>
       </c>
       <c r="O12" s="9">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>107</v>
+      </c>
+      <c r="R12">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -3720,13 +3881,19 @@
       </c>
       <c r="M13" s="6">
         <f t="shared" si="0"/>
-        <v>0.77922077922077926</v>
+        <v>0.52173913043478259</v>
       </c>
       <c r="O13" s="9">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>115</v>
+      </c>
+      <c r="R13">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3765,13 +3932,19 @@
       </c>
       <c r="M14" s="6">
         <f t="shared" si="0"/>
-        <v>0.76923076923076927</v>
+        <v>0.59405940594059403</v>
       </c>
       <c r="O14" s="9">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>101</v>
+      </c>
+      <c r="R14">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3810,13 +3983,19 @@
       </c>
       <c r="M15" s="6">
         <f t="shared" si="0"/>
-        <v>0.78947368421052633</v>
+        <v>0.625</v>
       </c>
       <c r="O15" s="9">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>96</v>
+      </c>
+      <c r="R15">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3855,13 +4034,19 @@
       </c>
       <c r="M16" s="6">
         <f t="shared" si="0"/>
-        <v>1.1538461538461537</v>
+        <v>1.0909090909090908</v>
       </c>
       <c r="P16">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>55</v>
+      </c>
+      <c r="R16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3905,8 +4090,14 @@
       <c r="P17">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>47</v>
+      </c>
+      <c r="R17">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -3945,13 +4136,19 @@
       </c>
       <c r="M18" s="6">
         <f t="shared" si="0"/>
-        <v>1.6216216216216217</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="P18">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>54</v>
+      </c>
+      <c r="R18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -3990,13 +4187,19 @@
       </c>
       <c r="M19" s="6">
         <f t="shared" si="0"/>
-        <v>1.4285714285714286</v>
+        <v>1.2</v>
       </c>
       <c r="P19">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>50</v>
+      </c>
+      <c r="R19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -4035,13 +4238,19 @@
       </c>
       <c r="M20" s="6">
         <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <v>1.5384615384615385</v>
       </c>
       <c r="P20">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>37</v>
+      </c>
+      <c r="R20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -4080,13 +4289,19 @@
       </c>
       <c r="M21" s="6">
         <f t="shared" si="0"/>
-        <v>1.4634146341463414</v>
+        <v>1.5384615384615385</v>
       </c>
       <c r="P21">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>27</v>
+      </c>
+      <c r="R21">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -4125,13 +4340,19 @@
       </c>
       <c r="M22" s="6">
         <f t="shared" si="0"/>
-        <v>1.3636363636363635</v>
+        <v>1.5384615384615385</v>
       </c>
       <c r="P22">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>39</v>
+      </c>
+      <c r="R22">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -4170,13 +4391,19 @@
       </c>
       <c r="M23" s="6">
         <f t="shared" si="0"/>
-        <v>1.875</v>
+        <v>1.5384615384615385</v>
       </c>
       <c r="P23">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>26</v>
+      </c>
+      <c r="R23">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -4214,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -4252,7 +4479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -4290,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -4328,7 +4555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -4366,7 +4593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -4404,7 +4631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -4442,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -4480,7 +4707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -4756,11 +4983,12 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:L1001 O12:O15">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>